<commit_message>
trimming data for 83 and 82 updated
</commit_message>
<xml_diff>
--- a/inventvmScripts/InnerLoop_Char/InnerLoop_Char2.xlsx
+++ b/inventvmScripts/InnerLoop_Char/InnerLoop_Char2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smplab\Documents\Franco\Inventvm\SW\inventvmScripts\InnerLoop_Char\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E69082-D012-4C6A-BDE6-B51C5703AA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{070E2519-EE42-427A-B2CC-E50DF61FB606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device1_4phases_HighSide_85C_OC" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,18 @@
     <sheet name="Device1_4phases_indcs_Low_sweep" sheetId="6" r:id="rId6"/>
     <sheet name="device1_reference" sheetId="7" r:id="rId7"/>
     <sheet name="device2_reference" sheetId="8" r:id="rId8"/>
+    <sheet name="Recovered_Sheet1" sheetId="9" r:id="rId9"/>
+    <sheet name="reference" sheetId="10" r:id="rId10"/>
+    <sheet name="Device2_4phases_LowSide_25C_OCP" sheetId="11" r:id="rId11"/>
+    <sheet name="Device2_4phases_LowSide_85C_OCP" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="32">
   <si>
     <t>ph1_OCPthershold</t>
   </si>
@@ -129,13 +134,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -161,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -214,11 +224,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -227,6 +252,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -842,6 +870,873 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:P6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.375</v>
+      </c>
+      <c r="C2">
+        <v>0.37280922999999988</v>
+      </c>
+      <c r="D2">
+        <v>-0.58420533333336522</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0.375</v>
+      </c>
+      <c r="G2">
+        <v>0.37091616999999988</v>
+      </c>
+      <c r="H2">
+        <v>-1.089021333333366</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0.375</v>
+      </c>
+      <c r="K2">
+        <v>0.39942022750000011</v>
+      </c>
+      <c r="L2">
+        <v>6.5120606666666818</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>0.375</v>
+      </c>
+      <c r="O2">
+        <v>0.39349107000000011</v>
+      </c>
+      <c r="P2">
+        <v>4.9309520000000138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5.5</v>
+      </c>
+      <c r="B3">
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="C3">
+        <v>0.41050148499999989</v>
+      </c>
+      <c r="D3">
+        <v>-0.48448848484849322</v>
+      </c>
+      <c r="E3">
+        <v>5.5</v>
+      </c>
+      <c r="F3">
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="G3">
+        <v>0.40870168000000012</v>
+      </c>
+      <c r="H3">
+        <v>-0.92080484848482691</v>
+      </c>
+      <c r="I3">
+        <v>5.5</v>
+      </c>
+      <c r="J3">
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="K3">
+        <v>0.43831542500000009</v>
+      </c>
+      <c r="L3">
+        <v>6.2582848484848768</v>
+      </c>
+      <c r="M3">
+        <v>5.5</v>
+      </c>
+      <c r="N3">
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="O3">
+        <v>0.43207431250000022</v>
+      </c>
+      <c r="P3">
+        <v>4.7452878787879254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.45</v>
+      </c>
+      <c r="C4">
+        <v>0.44809620249999987</v>
+      </c>
+      <c r="D4">
+        <v>-0.42306611111111703</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>0.45</v>
+      </c>
+      <c r="G4">
+        <v>0.44620336750000011</v>
+      </c>
+      <c r="H4">
+        <v>-0.8436961111110759</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>0.45</v>
+      </c>
+      <c r="K4">
+        <v>0.47698274249999989</v>
+      </c>
+      <c r="L4">
+        <v>5.9961649999999986</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>0.45</v>
+      </c>
+      <c r="O4">
+        <v>0.47070652000000002</v>
+      </c>
+      <c r="P4">
+        <v>4.6014488888889034</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6.5</v>
+      </c>
+      <c r="B5">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.48579854</v>
+      </c>
+      <c r="D5">
+        <v>-0.34901743589743339</v>
+      </c>
+      <c r="E5">
+        <v>6.5</v>
+      </c>
+      <c r="F5">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.48391460749999998</v>
+      </c>
+      <c r="H5">
+        <v>-0.73546512820511811</v>
+      </c>
+      <c r="I5">
+        <v>6.5</v>
+      </c>
+      <c r="J5">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="K5">
+        <v>0.51565634999999999</v>
+      </c>
+      <c r="L5">
+        <v>5.775661538461538</v>
+      </c>
+      <c r="M5">
+        <v>6.5</v>
+      </c>
+      <c r="N5">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="O5">
+        <v>0.50938931249999997</v>
+      </c>
+      <c r="P5">
+        <v>4.4901153846153807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="C6">
+        <v>0.52337803000000016</v>
+      </c>
+      <c r="D6">
+        <v>-0.30894666666664028</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.52180638500000009</v>
+      </c>
+      <c r="H6">
+        <v>-0.60830761904760522</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="K6">
+        <v>0.55445460750000009</v>
+      </c>
+      <c r="L6">
+        <v>5.6104014285714401</v>
+      </c>
+      <c r="M6">
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="O6">
+        <v>0.54806347750000017</v>
+      </c>
+      <c r="P6">
+        <v>4.3930433333333623</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:P6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4.9681870000000004</v>
+      </c>
+      <c r="C2">
+        <v>0.36982912600000001</v>
+      </c>
+      <c r="D2">
+        <v>1.378899733333331</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>4.6092409999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.36612354699999988</v>
+      </c>
+      <c r="H2">
+        <v>2.3670541333333501</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>5.4313339999999997</v>
+      </c>
+      <c r="K2">
+        <v>0.40717824549999998</v>
+      </c>
+      <c r="L2">
+        <v>-8.5808654666666602</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>5.4612660000000002</v>
+      </c>
+      <c r="O2">
+        <v>0.40256081075</v>
+      </c>
+      <c r="P2">
+        <v>-7.3495495333333327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5.5</v>
+      </c>
+      <c r="B3">
+        <v>5.4673559999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.40702206699999999</v>
+      </c>
+      <c r="D3">
+        <v>1.3279837575757549</v>
+      </c>
+      <c r="E3">
+        <v>5.5</v>
+      </c>
+      <c r="F3">
+        <v>5.0862939999999996</v>
+      </c>
+      <c r="G3">
+        <v>0.40357355299999997</v>
+      </c>
+      <c r="H3">
+        <v>2.1639871515151392</v>
+      </c>
+      <c r="I3">
+        <v>5.5</v>
+      </c>
+      <c r="J3">
+        <v>5.9373509999999996</v>
+      </c>
+      <c r="K3">
+        <v>0.44531329250000001</v>
+      </c>
+      <c r="L3">
+        <v>-7.9547375757575853</v>
+      </c>
+      <c r="M3">
+        <v>5.5</v>
+      </c>
+      <c r="N3">
+        <v>5.9903060000000004</v>
+      </c>
+      <c r="O3">
+        <v>0.44178498775000002</v>
+      </c>
+      <c r="P3">
+        <v>-7.0993909696969686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5.9713130000000003</v>
+      </c>
+      <c r="C4">
+        <v>0.44456514400000002</v>
+      </c>
+      <c r="D4">
+        <v>1.2077457777777629</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>5.5662849999999997</v>
+      </c>
+      <c r="G4">
+        <v>0.44131063199999998</v>
+      </c>
+      <c r="H4">
+        <v>1.9309706666666611</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>6.4564339999999998</v>
+      </c>
+      <c r="K4">
+        <v>0.48430164074999998</v>
+      </c>
+      <c r="L4">
+        <v>-7.6225868333333402</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>6.4614180000000001</v>
+      </c>
+      <c r="O4">
+        <v>0.47663228499999999</v>
+      </c>
+      <c r="P4">
+        <v>-5.9182855555555633</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6.5</v>
+      </c>
+      <c r="B5">
+        <v>6.4733390000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.48196829125000001</v>
+      </c>
+      <c r="D5">
+        <v>1.1347094871794821</v>
+      </c>
+      <c r="E5">
+        <v>6.5</v>
+      </c>
+      <c r="F5">
+        <v>6.0412569999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.4785702335</v>
+      </c>
+      <c r="H5">
+        <v>1.8317469743589729</v>
+      </c>
+      <c r="I5">
+        <v>6.5</v>
+      </c>
+      <c r="J5">
+        <v>6.9614050000000001</v>
+      </c>
+      <c r="K5">
+        <v>0.52227899924999999</v>
+      </c>
+      <c r="L5">
+        <v>-7.1341536923076916</v>
+      </c>
+      <c r="M5">
+        <v>6.5</v>
+      </c>
+      <c r="N5">
+        <v>6.9994120000000004</v>
+      </c>
+      <c r="O5">
+        <v>0.51638801025000003</v>
+      </c>
+      <c r="P5">
+        <v>-5.9257456923077001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>6.9564019999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.51796189449999996</v>
+      </c>
+      <c r="D6">
+        <v>1.3405915238095349</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>6.534402</v>
+      </c>
+      <c r="G6">
+        <v>0.51716196700000006</v>
+      </c>
+      <c r="H6">
+        <v>1.4929586666666601</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>7.4774409999999998</v>
+      </c>
+      <c r="K6">
+        <v>0.56094452699999997</v>
+      </c>
+      <c r="L6">
+        <v>-6.8465765714285611</v>
+      </c>
+      <c r="M6">
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <v>7.4994319999999997</v>
+      </c>
+      <c r="O6">
+        <v>0.55330300975000002</v>
+      </c>
+      <c r="P6">
+        <v>-5.3910494761904753</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5.0362749999999998</v>
+      </c>
+      <c r="C2">
+        <v>0.3711703415</v>
+      </c>
+      <c r="D2">
+        <v>1.021242266666667</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>4.7021660000000001</v>
+      </c>
+      <c r="G2">
+        <v>0.36858063824999998</v>
+      </c>
+      <c r="H2">
+        <v>1.7118297999999901</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>5.5223550000000001</v>
+      </c>
+      <c r="K2">
+        <v>0.40978423274999998</v>
+      </c>
+      <c r="L2">
+        <v>-9.2757954000000087</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5.5</v>
+      </c>
+      <c r="B3">
+        <v>5.5312710000000003</v>
+      </c>
+      <c r="C3">
+        <v>0.40808164349999998</v>
+      </c>
+      <c r="D3">
+        <v>1.0711167272727271</v>
+      </c>
+      <c r="E3">
+        <v>5.5</v>
+      </c>
+      <c r="F3">
+        <v>5.1802320000000002</v>
+      </c>
+      <c r="G3">
+        <v>0.40600406174999998</v>
+      </c>
+      <c r="H3">
+        <v>1.5747729090909091</v>
+      </c>
+      <c r="I3">
+        <v>5.5</v>
+      </c>
+      <c r="J3">
+        <v>6.0383079999999998</v>
+      </c>
+      <c r="K3">
+        <v>0.44862242875000002</v>
+      </c>
+      <c r="L3">
+        <v>-8.7569524242424226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>6.0243190000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.44519381224999999</v>
+      </c>
+      <c r="D4">
+        <v>1.0680417222222149</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>5.6563330000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.44332979550000001</v>
+      </c>
+      <c r="H4">
+        <v>1.482267666666667</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>6.5284219999999999</v>
+      </c>
+      <c r="K4">
+        <v>0.48538813824999999</v>
+      </c>
+      <c r="L4">
+        <v>-7.8640307222222301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6.5</v>
+      </c>
+      <c r="B5">
+        <v>6.5374090000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.48346520050000003</v>
+      </c>
+      <c r="D5">
+        <v>0.82765117948718336</v>
+      </c>
+      <c r="E5">
+        <v>6.5</v>
+      </c>
+      <c r="F5">
+        <v>6.1443510000000003</v>
+      </c>
+      <c r="G5">
+        <v>0.48152139049999998</v>
+      </c>
+      <c r="H5">
+        <v>1.2263814358974381</v>
+      </c>
+      <c r="I5">
+        <v>6.5</v>
+      </c>
+      <c r="J5">
+        <v>7.0034000000000001</v>
+      </c>
+      <c r="K5">
+        <v>0.52161448050000003</v>
+      </c>
+      <c r="L5">
+        <v>-6.9978421538461637</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>7.0354260000000002</v>
+      </c>
+      <c r="C6">
+        <v>0.52044081349999993</v>
+      </c>
+      <c r="D6">
+        <v>0.86841647619049323</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>6.6213639999999998</v>
+      </c>
+      <c r="G6">
+        <v>0.518771235</v>
+      </c>
+      <c r="H6">
+        <v>1.186431428571433</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>7.5084900000000001</v>
+      </c>
+      <c r="K6">
+        <v>7.763805682500001E-2</v>
+      </c>
+      <c r="L6">
+        <v>85.211798700000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1"/>
@@ -9589,7 +10484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
@@ -9898,4 +10793,67 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>